<commit_message>
Implement Canvasing Input Form and update Sidebar
</commit_message>
<xml_diff>
--- a/Master Template.xlsx
+++ b/Master Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\to do list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D821236-64A0-4882-9AE6-F8746C8989EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F647E916-587F-49B4-8CBD-E1761C676012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6859" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6915" uniqueCount="317">
   <si>
     <t>Nama</t>
   </si>
@@ -1306,6 +1306,9 @@
   </si>
   <si>
     <t>Relawan Guru</t>
+  </si>
+  <si>
+    <t>Reporting</t>
   </si>
 </sst>
 </file>
@@ -1690,10 +1693,10 @@
   <dimension ref="A1:S628"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B167" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="C108" sqref="C108:C184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2359,6 +2362,9 @@
       <c r="B16" t="s">
         <v>32</v>
       </c>
+      <c r="C16" t="s">
+        <v>316</v>
+      </c>
       <c r="D16" t="s">
         <v>33</v>
       </c>
@@ -2403,6 +2409,9 @@
       <c r="B17" t="s">
         <v>32</v>
       </c>
+      <c r="C17" t="s">
+        <v>316</v>
+      </c>
       <c r="D17" t="s">
         <v>34</v>
       </c>
@@ -2447,6 +2456,9 @@
       <c r="B18" t="s">
         <v>32</v>
       </c>
+      <c r="C18" t="s">
+        <v>316</v>
+      </c>
       <c r="D18" t="s">
         <v>35</v>
       </c>
@@ -2491,6 +2503,9 @@
       <c r="B19" t="s">
         <v>32</v>
       </c>
+      <c r="C19" t="s">
+        <v>316</v>
+      </c>
       <c r="D19" t="s">
         <v>36</v>
       </c>
@@ -2535,6 +2550,9 @@
       <c r="B20" t="s">
         <v>32</v>
       </c>
+      <c r="C20" t="s">
+        <v>316</v>
+      </c>
       <c r="D20" t="s">
         <v>37</v>
       </c>
@@ -2579,6 +2597,9 @@
       <c r="B21" t="s">
         <v>32</v>
       </c>
+      <c r="C21" t="s">
+        <v>316</v>
+      </c>
       <c r="D21" t="s">
         <v>38</v>
       </c>
@@ -2616,13 +2637,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>31</v>
       </c>
       <c r="B22" t="s">
         <v>32</v>
       </c>
+      <c r="C22" t="s">
+        <v>316</v>
+      </c>
       <c r="D22" t="s">
         <v>39</v>
       </c>
@@ -2660,13 +2684,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" t="s">
         <v>32</v>
       </c>
+      <c r="C23" t="s">
+        <v>316</v>
+      </c>
       <c r="D23" t="s">
         <v>39</v>
       </c>
@@ -2704,13 +2731,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>31</v>
       </c>
       <c r="B24" t="s">
         <v>32</v>
       </c>
+      <c r="C24" t="s">
+        <v>316</v>
+      </c>
       <c r="D24" t="s">
         <v>36</v>
       </c>
@@ -2748,13 +2778,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>32</v>
       </c>
+      <c r="C25" t="s">
+        <v>316</v>
+      </c>
       <c r="D25" t="s">
         <v>40</v>
       </c>
@@ -2792,13 +2825,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>32</v>
       </c>
+      <c r="C26" t="s">
+        <v>316</v>
+      </c>
       <c r="D26" t="s">
         <v>38</v>
       </c>
@@ -2836,7 +2872,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -2883,7 +2919,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -2930,7 +2966,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -2977,7 +3013,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -3024,7 +3060,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -3071,7 +3107,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -3118,7 +3154,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -3165,7 +3201,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -3212,7 +3248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -3259,7 +3295,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -3306,7 +3342,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -3353,7 +3389,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -3400,7 +3436,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -3447,7 +3483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -3494,7 +3530,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -3541,7 +3577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -3588,7 +3624,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -3635,7 +3671,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -3682,7 +3718,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -3729,7 +3765,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -3870,7 +3906,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -4005,7 +4041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -4046,7 +4082,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -4087,7 +4123,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -4128,7 +4164,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="55" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -4175,7 +4211,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="56" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -4216,7 +4252,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="57" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -4263,7 +4299,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -4310,7 +4346,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="59" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>19</v>
       </c>
@@ -4354,7 +4390,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="60" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>19</v>
       </c>
@@ -4398,7 +4434,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="61" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
@@ -4442,7 +4478,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="62" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>107</v>
       </c>
@@ -4486,7 +4522,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>19</v>
       </c>
@@ -4496,6 +4532,9 @@
       <c r="C63" t="s">
         <v>117</v>
       </c>
+      <c r="D63" t="s">
+        <v>117</v>
+      </c>
       <c r="F63" t="s">
         <v>26</v>
       </c>
@@ -4530,7 +4569,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="64" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>107</v>
       </c>
@@ -4540,6 +4579,9 @@
       <c r="C64" t="s">
         <v>118</v>
       </c>
+      <c r="D64" t="s">
+        <v>118</v>
+      </c>
       <c r="F64" t="s">
         <v>26</v>
       </c>
@@ -4574,7 +4616,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>107</v>
       </c>
@@ -4584,6 +4626,9 @@
       <c r="C65" t="s">
         <v>118</v>
       </c>
+      <c r="D65" t="s">
+        <v>118</v>
+      </c>
       <c r="F65" t="s">
         <v>26</v>
       </c>
@@ -4618,7 +4663,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>107</v>
       </c>
@@ -4628,6 +4673,9 @@
       <c r="C66" t="s">
         <v>118</v>
       </c>
+      <c r="D66" t="s">
+        <v>118</v>
+      </c>
       <c r="F66" t="s">
         <v>26</v>
       </c>
@@ -4662,7 +4710,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>107</v>
       </c>
@@ -4672,6 +4720,9 @@
       <c r="C67" t="s">
         <v>118</v>
       </c>
+      <c r="D67" t="s">
+        <v>118</v>
+      </c>
       <c r="F67" t="s">
         <v>26</v>
       </c>
@@ -4706,7 +4757,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="68" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>107</v>
       </c>
@@ -4716,6 +4767,9 @@
       <c r="C68" t="s">
         <v>118</v>
       </c>
+      <c r="D68" t="s">
+        <v>118</v>
+      </c>
       <c r="F68" t="s">
         <v>26</v>
       </c>
@@ -4750,7 +4804,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="69" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>107</v>
       </c>
@@ -4760,6 +4814,9 @@
       <c r="C69" t="s">
         <v>118</v>
       </c>
+      <c r="D69" t="s">
+        <v>118</v>
+      </c>
       <c r="F69" t="s">
         <v>26</v>
       </c>
@@ -4794,7 +4851,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="70" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>107</v>
       </c>
@@ -4804,6 +4861,9 @@
       <c r="C70" t="s">
         <v>118</v>
       </c>
+      <c r="D70" t="s">
+        <v>118</v>
+      </c>
       <c r="F70" t="s">
         <v>26</v>
       </c>
@@ -4838,7 +4898,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="71" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>107</v>
       </c>
@@ -4848,6 +4908,9 @@
       <c r="C71" t="s">
         <v>118</v>
       </c>
+      <c r="D71" t="s">
+        <v>118</v>
+      </c>
       <c r="F71" t="s">
         <v>26</v>
       </c>
@@ -4882,7 +4945,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>107</v>
       </c>
@@ -4892,6 +4955,9 @@
       <c r="C72" t="s">
         <v>118</v>
       </c>
+      <c r="D72" t="s">
+        <v>118</v>
+      </c>
       <c r="F72" t="s">
         <v>26</v>
       </c>
@@ -4926,7 +4992,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="73" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>107</v>
       </c>
@@ -4936,6 +5002,9 @@
       <c r="C73" t="s">
         <v>118</v>
       </c>
+      <c r="D73" t="s">
+        <v>118</v>
+      </c>
       <c r="F73" t="s">
         <v>26</v>
       </c>
@@ -4970,7 +5039,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>107</v>
       </c>
@@ -4980,6 +5049,9 @@
       <c r="C74" t="s">
         <v>118</v>
       </c>
+      <c r="D74" t="s">
+        <v>118</v>
+      </c>
       <c r="F74" t="s">
         <v>26</v>
       </c>
@@ -5014,7 +5086,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>107</v>
       </c>
@@ -5024,6 +5096,9 @@
       <c r="C75" t="s">
         <v>118</v>
       </c>
+      <c r="D75" t="s">
+        <v>118</v>
+      </c>
       <c r="F75" t="s">
         <v>26</v>
       </c>
@@ -5058,7 +5133,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="76" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>115</v>
       </c>
@@ -5068,6 +5143,9 @@
       <c r="C76" t="s">
         <v>119</v>
       </c>
+      <c r="D76" t="s">
+        <v>119</v>
+      </c>
       <c r="F76" t="s">
         <v>26</v>
       </c>
@@ -5102,7 +5180,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>115</v>
       </c>
@@ -5112,6 +5190,9 @@
       <c r="C77" t="s">
         <v>119</v>
       </c>
+      <c r="D77" t="s">
+        <v>119</v>
+      </c>
       <c r="F77" t="s">
         <v>26</v>
       </c>
@@ -5146,7 +5227,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="78" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>115</v>
       </c>
@@ -5156,6 +5237,9 @@
       <c r="C78" t="s">
         <v>119</v>
       </c>
+      <c r="D78" t="s">
+        <v>119</v>
+      </c>
       <c r="F78" t="s">
         <v>26</v>
       </c>
@@ -5190,7 +5274,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="79" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>115</v>
       </c>
@@ -5200,6 +5284,9 @@
       <c r="C79" t="s">
         <v>119</v>
       </c>
+      <c r="D79" t="s">
+        <v>119</v>
+      </c>
       <c r="F79" t="s">
         <v>26</v>
       </c>
@@ -5234,7 +5321,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="80" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>115</v>
       </c>
@@ -5244,6 +5331,9 @@
       <c r="C80" t="s">
         <v>119</v>
       </c>
+      <c r="D80" t="s">
+        <v>119</v>
+      </c>
       <c r="F80" t="s">
         <v>26</v>
       </c>
@@ -5278,7 +5368,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="81" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>115</v>
       </c>
@@ -5288,6 +5378,9 @@
       <c r="C81" t="s">
         <v>119</v>
       </c>
+      <c r="D81" t="s">
+        <v>119</v>
+      </c>
       <c r="F81" t="s">
         <v>26</v>
       </c>
@@ -5322,7 +5415,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="82" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>115</v>
       </c>
@@ -5332,6 +5425,9 @@
       <c r="C82" t="s">
         <v>119</v>
       </c>
+      <c r="D82" t="s">
+        <v>119</v>
+      </c>
       <c r="F82" t="s">
         <v>26</v>
       </c>
@@ -5366,7 +5462,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>115</v>
       </c>
@@ -5376,6 +5472,9 @@
       <c r="C83" t="s">
         <v>119</v>
       </c>
+      <c r="D83" t="s">
+        <v>119</v>
+      </c>
       <c r="F83" t="s">
         <v>26</v>
       </c>
@@ -5410,7 +5509,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="84" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>115</v>
       </c>
@@ -5420,6 +5519,9 @@
       <c r="C84" t="s">
         <v>119</v>
       </c>
+      <c r="D84" t="s">
+        <v>119</v>
+      </c>
       <c r="F84" t="s">
         <v>26</v>
       </c>
@@ -5454,7 +5556,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="85" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>115</v>
       </c>
@@ -5464,6 +5566,9 @@
       <c r="C85" t="s">
         <v>119</v>
       </c>
+      <c r="D85" t="s">
+        <v>119</v>
+      </c>
       <c r="F85" t="s">
         <v>26</v>
       </c>
@@ -5498,7 +5603,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="86" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>115</v>
       </c>
@@ -5508,6 +5613,9 @@
       <c r="C86" t="s">
         <v>119</v>
       </c>
+      <c r="D86" t="s">
+        <v>119</v>
+      </c>
       <c r="F86" t="s">
         <v>26</v>
       </c>
@@ -5542,7 +5650,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="87" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>115</v>
       </c>
@@ -5552,6 +5660,9 @@
       <c r="C87" t="s">
         <v>119</v>
       </c>
+      <c r="D87" t="s">
+        <v>119</v>
+      </c>
       <c r="F87" t="s">
         <v>26</v>
       </c>
@@ -5586,7 +5697,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="88" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>19</v>
       </c>
@@ -5596,6 +5707,9 @@
       <c r="C88" t="s">
         <v>121</v>
       </c>
+      <c r="D88" t="s">
+        <v>121</v>
+      </c>
       <c r="F88" t="s">
         <v>26</v>
       </c>
@@ -5630,7 +5744,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="89" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>19</v>
       </c>
@@ -5640,6 +5754,9 @@
       <c r="C89" t="s">
         <v>121</v>
       </c>
+      <c r="D89" t="s">
+        <v>121</v>
+      </c>
       <c r="F89" t="s">
         <v>26</v>
       </c>
@@ -5674,7 +5791,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="90" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>19</v>
       </c>
@@ -5684,6 +5801,9 @@
       <c r="C90" t="s">
         <v>122</v>
       </c>
+      <c r="D90" t="s">
+        <v>122</v>
+      </c>
       <c r="F90" t="s">
         <v>26</v>
       </c>
@@ -5718,7 +5838,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="91" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>107</v>
       </c>
@@ -5728,6 +5848,9 @@
       <c r="C91" t="s">
         <v>121</v>
       </c>
+      <c r="D91" t="s">
+        <v>121</v>
+      </c>
       <c r="F91" t="s">
         <v>26</v>
       </c>
@@ -5762,7 +5885,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>107</v>
       </c>
@@ -5772,6 +5895,9 @@
       <c r="C92" t="s">
         <v>121</v>
       </c>
+      <c r="D92" t="s">
+        <v>121</v>
+      </c>
       <c r="F92" t="s">
         <v>26</v>
       </c>
@@ -5806,7 +5932,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="93" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>107</v>
       </c>
@@ -5816,6 +5942,9 @@
       <c r="C93" t="s">
         <v>122</v>
       </c>
+      <c r="D93" t="s">
+        <v>122</v>
+      </c>
       <c r="F93" t="s">
         <v>26</v>
       </c>
@@ -5850,7 +5979,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="94" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>107</v>
       </c>
@@ -5860,6 +5989,9 @@
       <c r="C94" t="s">
         <v>124</v>
       </c>
+      <c r="D94" t="s">
+        <v>124</v>
+      </c>
       <c r="F94" t="s">
         <v>26</v>
       </c>
@@ -5894,7 +6026,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="95" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>107</v>
       </c>
@@ -5904,6 +6036,9 @@
       <c r="C95" t="s">
         <v>124</v>
       </c>
+      <c r="D95" t="s">
+        <v>124</v>
+      </c>
       <c r="F95" t="s">
         <v>26</v>
       </c>
@@ -5938,7 +6073,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="96" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>107</v>
       </c>
@@ -5948,6 +6083,9 @@
       <c r="C96" t="s">
         <v>126</v>
       </c>
+      <c r="D96" t="s">
+        <v>126</v>
+      </c>
       <c r="F96" t="s">
         <v>26</v>
       </c>
@@ -5982,7 +6120,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="97" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>107</v>
       </c>
@@ -5992,6 +6130,9 @@
       <c r="C97" t="s">
         <v>126</v>
       </c>
+      <c r="D97" t="s">
+        <v>126</v>
+      </c>
       <c r="F97" t="s">
         <v>26</v>
       </c>
@@ -6026,7 +6167,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="98" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>107</v>
       </c>
@@ -6036,6 +6177,9 @@
       <c r="C98" t="s">
         <v>126</v>
       </c>
+      <c r="D98" t="s">
+        <v>126</v>
+      </c>
       <c r="F98" t="s">
         <v>26</v>
       </c>
@@ -6070,7 +6214,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="99" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>107</v>
       </c>
@@ -6080,6 +6224,9 @@
       <c r="C99" t="s">
         <v>126</v>
       </c>
+      <c r="D99" t="s">
+        <v>126</v>
+      </c>
       <c r="F99" t="s">
         <v>26</v>
       </c>
@@ -6114,7 +6261,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="100" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>107</v>
       </c>
@@ -6124,6 +6271,9 @@
       <c r="C100" t="s">
         <v>126</v>
       </c>
+      <c r="D100" t="s">
+        <v>126</v>
+      </c>
       <c r="F100" t="s">
         <v>26</v>
       </c>
@@ -6158,7 +6308,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="101" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -6168,6 +6318,9 @@
       <c r="C101" t="s">
         <v>126</v>
       </c>
+      <c r="D101" t="s">
+        <v>126</v>
+      </c>
       <c r="F101" t="s">
         <v>26</v>
       </c>
@@ -6202,7 +6355,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="102" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>107</v>
       </c>
@@ -6212,6 +6365,9 @@
       <c r="C102" t="s">
         <v>126</v>
       </c>
+      <c r="D102" t="s">
+        <v>126</v>
+      </c>
       <c r="F102" t="s">
         <v>26</v>
       </c>
@@ -6246,7 +6402,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="103" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>107</v>
       </c>
@@ -6256,6 +6412,9 @@
       <c r="C103" t="s">
         <v>126</v>
       </c>
+      <c r="D103" t="s">
+        <v>126</v>
+      </c>
       <c r="F103" t="s">
         <v>26</v>
       </c>
@@ -6290,7 +6449,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>107</v>
       </c>
@@ -6300,6 +6459,9 @@
       <c r="C104" t="s">
         <v>126</v>
       </c>
+      <c r="D104" t="s">
+        <v>126</v>
+      </c>
       <c r="F104" t="s">
         <v>26</v>
       </c>
@@ -6334,7 +6496,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="105" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>107</v>
       </c>
@@ -6344,6 +6506,9 @@
       <c r="C105" t="s">
         <v>126</v>
       </c>
+      <c r="D105" t="s">
+        <v>126</v>
+      </c>
       <c r="F105" t="s">
         <v>26</v>
       </c>
@@ -6378,7 +6543,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="106" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>107</v>
       </c>
@@ -6388,6 +6553,9 @@
       <c r="C106" t="s">
         <v>126</v>
       </c>
+      <c r="D106" t="s">
+        <v>126</v>
+      </c>
       <c r="F106" t="s">
         <v>26</v>
       </c>
@@ -6422,7 +6590,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="107" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -6432,6 +6600,9 @@
       <c r="C107" t="s">
         <v>126</v>
       </c>
+      <c r="D107" t="s">
+        <v>126</v>
+      </c>
       <c r="F107" t="s">
         <v>26</v>
       </c>
@@ -6466,7 +6637,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="108" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -6510,7 +6681,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="109" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>107</v>
       </c>
@@ -6554,7 +6725,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -6598,7 +6769,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>107</v>
       </c>
@@ -6642,7 +6813,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>107</v>
       </c>
@@ -6686,7 +6857,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>107</v>
       </c>
@@ -6730,7 +6901,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>107</v>
       </c>
@@ -6774,7 +6945,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>107</v>
       </c>
@@ -6818,7 +6989,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>107</v>
       </c>
@@ -6862,7 +7033,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>107</v>
       </c>
@@ -6906,7 +7077,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>107</v>
       </c>
@@ -6950,7 +7121,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>107</v>
       </c>
@@ -6994,7 +7165,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>107</v>
       </c>
@@ -7038,7 +7209,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="121" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>107</v>
       </c>
@@ -7082,7 +7253,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>107</v>
       </c>
@@ -7126,7 +7297,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>115</v>
       </c>
@@ -7170,7 +7341,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="124" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>115</v>
       </c>
@@ -7214,7 +7385,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>115</v>
       </c>
@@ -7258,7 +7429,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>115</v>
       </c>
@@ -7302,7 +7473,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="127" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>115</v>
       </c>
@@ -7346,7 +7517,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>115</v>
       </c>
@@ -7390,7 +7561,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>115</v>
       </c>
@@ -7434,7 +7605,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="130" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>115</v>
       </c>
@@ -7478,7 +7649,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>115</v>
       </c>
@@ -7522,7 +7693,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>115</v>
       </c>
@@ -7566,7 +7737,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>115</v>
       </c>
@@ -7610,7 +7781,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>115</v>
       </c>
@@ -7654,7 +7825,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>115</v>
       </c>
@@ -7698,7 +7869,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>115</v>
       </c>
@@ -7742,7 +7913,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>115</v>
       </c>
@@ -7786,7 +7957,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>115</v>
       </c>
@@ -7830,7 +8001,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="139" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>115</v>
       </c>
@@ -7874,7 +8045,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>115</v>
       </c>
@@ -7918,7 +8089,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>115</v>
       </c>
@@ -7962,7 +8133,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="142" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>115</v>
       </c>
@@ -8006,7 +8177,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>115</v>
       </c>
@@ -8050,7 +8221,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>115</v>
       </c>
@@ -8094,7 +8265,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>115</v>
       </c>
@@ -8138,7 +8309,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>115</v>
       </c>
@@ -8182,7 +8353,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>115</v>
       </c>
@@ -8226,7 +8397,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>115</v>
       </c>
@@ -8270,7 +8441,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>115</v>
       </c>
@@ -8314,7 +8485,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>115</v>
       </c>
@@ -8358,7 +8529,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>115</v>
       </c>
@@ -8402,7 +8573,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>115</v>
       </c>
@@ -8446,7 +8617,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>115</v>
       </c>
@@ -8490,7 +8661,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>115</v>
       </c>
@@ -8534,7 +8705,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>115</v>
       </c>
@@ -8578,7 +8749,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>115</v>
       </c>
@@ -8622,7 +8793,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>115</v>
       </c>
@@ -8666,7 +8837,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>115</v>
       </c>
@@ -8710,7 +8881,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>115</v>
       </c>
@@ -8754,7 +8925,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>115</v>
       </c>
@@ -8798,7 +8969,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>115</v>
       </c>
@@ -8836,7 +9007,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>115</v>
       </c>
@@ -8874,7 +9045,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>115</v>
       </c>
@@ -8912,7 +9083,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>19</v>
       </c>
@@ -8950,7 +9121,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>19</v>
       </c>
@@ -8988,7 +9159,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>19</v>
       </c>
@@ -9026,7 +9197,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>19</v>
       </c>
@@ -9064,7 +9235,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>19</v>
       </c>
@@ -9102,7 +9273,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>19</v>
       </c>
@@ -9140,7 +9311,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>19</v>
       </c>
@@ -9178,7 +9349,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>19</v>
       </c>
@@ -9216,7 +9387,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="172" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>19</v>
       </c>
@@ -9254,7 +9425,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>19</v>
       </c>
@@ -9292,7 +9463,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>134</v>
       </c>
@@ -9330,7 +9501,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>134</v>
       </c>
@@ -9368,7 +9539,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>134</v>
       </c>
@@ -9406,7 +9577,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>134</v>
       </c>
@@ -9444,7 +9615,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>134</v>
       </c>
@@ -9482,7 +9653,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>134</v>
       </c>
@@ -9520,7 +9691,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>134</v>
       </c>
@@ -9558,7 +9729,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>134</v>
       </c>
@@ -9596,7 +9767,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>134</v>
       </c>
@@ -9634,7 +9805,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>134</v>
       </c>
@@ -9672,7 +9843,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="184" spans="1:18" hidden="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>134</v>
       </c>
@@ -30643,19 +30814,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:S628" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Iik Iksandi"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="6">
       <filters>
         <dateGroupItem year="2026" month="1" dateTimeGrouping="month"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="16">
-      <filters>
-        <filter val="HRD"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>